<commit_message>
added column in import page
</commit_message>
<xml_diff>
--- a/docs/data sample/2022年市场监督管理局-复审.xlsx
+++ b/docs/data sample/2022年市场监督管理局-复审.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4009" uniqueCount="1208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4008" uniqueCount="1208">
   <si>
     <t>序号</t>
   </si>
@@ -4921,8 +4921,8 @@
   <sheetPr/>
   <dimension ref="A1:R358"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A344" workbookViewId="0">
-      <selection activeCell="K363" sqref="K363"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="K361" sqref="K361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -20198,9 +20198,7 @@
       <c r="H358" s="9"/>
       <c r="I358" s="9"/>
       <c r="J358" s="9"/>
-      <c r="K358" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="K358" s="9"/>
       <c r="L358" s="9" t="s">
         <v>1188</v>
       </c>

</xml_diff>